<commit_message>
end of play - Friday
</commit_message>
<xml_diff>
--- a/formal/UNAIDS/results/DRC/DRC.xlsx
+++ b/formal/UNAIDS/results/DRC/DRC.xlsx
@@ -54,34 +54,34 @@
     <t>DRC</t>
   </si>
   <si>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
     <t>0.39</t>
   </si>
   <si>
-    <t>0.81</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
-    <t>0.59</t>
-  </si>
-  <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>max_error = 0.8, min_number = 500, treat all from 2016</t>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>max_error = 0.15, min_number = 1000</t>
   </si>
   <si>
     <t>PLHIV</t>
@@ -129,94 +129,94 @@
     <t>PLHIV Virally Suppressed upper 95% CI</t>
   </si>
   <si>
-    <t>384078</t>
-  </si>
-  <si>
-    <t>109787</t>
-  </si>
-  <si>
-    <t>75683</t>
-  </si>
-  <si>
-    <t>75208</t>
-  </si>
-  <si>
-    <t>67083</t>
-  </si>
-  <si>
-    <t>268848</t>
-  </si>
-  <si>
-    <t>67531</t>
-  </si>
-  <si>
-    <t>34768</t>
-  </si>
-  <si>
-    <t>34506</t>
-  </si>
-  <si>
-    <t>32336</t>
-  </si>
-  <si>
-    <t>545413</t>
-  </si>
-  <si>
-    <t>152345</t>
-  </si>
-  <si>
-    <t>114508</t>
-  </si>
-  <si>
-    <t>113992</t>
-  </si>
-  <si>
-    <t>99692</t>
-  </si>
-  <si>
-    <t>378231</t>
-  </si>
-  <si>
-    <t>142236</t>
-  </si>
-  <si>
-    <t>118183</t>
-  </si>
-  <si>
-    <t>118062</t>
-  </si>
-  <si>
-    <t>105801</t>
-  </si>
-  <si>
-    <t>271796</t>
-  </si>
-  <si>
-    <t>71052</t>
-  </si>
-  <si>
-    <t>40881</t>
-  </si>
-  <si>
-    <t>40771</t>
-  </si>
-  <si>
-    <t>37680</t>
-  </si>
-  <si>
-    <t>503646</t>
-  </si>
-  <si>
-    <t>217638</t>
-  </si>
-  <si>
-    <t>194287</t>
-  </si>
-  <si>
-    <t>194180</t>
-  </si>
-  <si>
-    <t>171049</t>
+    <t>393501</t>
+  </si>
+  <si>
+    <t>165837</t>
+  </si>
+  <si>
+    <t>98597</t>
+  </si>
+  <si>
+    <t>97990</t>
+  </si>
+  <si>
+    <t>36986</t>
+  </si>
+  <si>
+    <t>348228</t>
+  </si>
+  <si>
+    <t>128922</t>
+  </si>
+  <si>
+    <t>75035</t>
+  </si>
+  <si>
+    <t>74501</t>
+  </si>
+  <si>
+    <t>6021</t>
+  </si>
+  <si>
+    <t>444139</t>
+  </si>
+  <si>
+    <t>200101</t>
+  </si>
+  <si>
+    <t>120024</t>
+  </si>
+  <si>
+    <t>119082</t>
+  </si>
+  <si>
+    <t>74557</t>
+  </si>
+  <si>
+    <t>353322</t>
+  </si>
+  <si>
+    <t>206972</t>
+  </si>
+  <si>
+    <t>153230</t>
+  </si>
+  <si>
+    <t>152890</t>
+  </si>
+  <si>
+    <t>61210</t>
+  </si>
+  <si>
+    <t>305348</t>
+  </si>
+  <si>
+    <t>166117</t>
+  </si>
+  <si>
+    <t>116445</t>
+  </si>
+  <si>
+    <t>115914</t>
+  </si>
+  <si>
+    <t>9767</t>
+  </si>
+  <si>
+    <t>401548</t>
+  </si>
+  <si>
+    <t>245245</t>
+  </si>
+  <si>
+    <t>190544</t>
+  </si>
+  <si>
+    <t>190204</t>
+  </si>
+  <si>
+    <t>123451</t>
   </si>
   <si>
     <t>2015</t>
@@ -264,94 +264,94 @@
     <t>2019 upper 95% CI</t>
   </si>
   <si>
-    <t>12294</t>
-  </si>
-  <si>
-    <t>13619</t>
-  </si>
-  <si>
-    <t>15701</t>
-  </si>
-  <si>
-    <t>17191</t>
-  </si>
-  <si>
-    <t>18360</t>
-  </si>
-  <si>
-    <t>8535</t>
-  </si>
-  <si>
-    <t>9723</t>
-  </si>
-  <si>
-    <t>10643</t>
-  </si>
-  <si>
-    <t>11256</t>
-  </si>
-  <si>
-    <t>11270</t>
-  </si>
-  <si>
-    <t>16405</t>
-  </si>
-  <si>
-    <t>19689</t>
-  </si>
-  <si>
-    <t>23889</t>
-  </si>
-  <si>
-    <t>26711</t>
-  </si>
-  <si>
-    <t>29956</t>
-  </si>
-  <si>
-    <t>15422</t>
-  </si>
-  <si>
-    <t>16057</t>
-  </si>
-  <si>
-    <t>16463</t>
-  </si>
-  <si>
-    <t>16718</t>
-  </si>
-  <si>
-    <t>16835</t>
-  </si>
-  <si>
-    <t>9449</t>
-  </si>
-  <si>
-    <t>9538</t>
-  </si>
-  <si>
-    <t>10017</t>
-  </si>
-  <si>
-    <t>9822</t>
-  </si>
-  <si>
-    <t>9446</t>
-  </si>
-  <si>
-    <t>21355</t>
-  </si>
-  <si>
-    <t>22616</t>
-  </si>
-  <si>
-    <t>23764</t>
-  </si>
-  <si>
-    <t>24091</t>
-  </si>
-  <si>
-    <t>25695</t>
+    <t>17897</t>
+  </si>
+  <si>
+    <t>19976</t>
+  </si>
+  <si>
+    <t>21315</t>
+  </si>
+  <si>
+    <t>21820</t>
+  </si>
+  <si>
+    <t>22079</t>
+  </si>
+  <si>
+    <t>14633</t>
+  </si>
+  <si>
+    <t>15515</t>
+  </si>
+  <si>
+    <t>16613</t>
+  </si>
+  <si>
+    <t>17092</t>
+  </si>
+  <si>
+    <t>17506</t>
+  </si>
+  <si>
+    <t>21769</t>
+  </si>
+  <si>
+    <t>25113</t>
+  </si>
+  <si>
+    <t>26309</t>
+  </si>
+  <si>
+    <t>26651</t>
+  </si>
+  <si>
+    <t>26557</t>
+  </si>
+  <si>
+    <t>15107</t>
+  </si>
+  <si>
+    <t>15164</t>
+  </si>
+  <si>
+    <t>15060</t>
+  </si>
+  <si>
+    <t>14903</t>
+  </si>
+  <si>
+    <t>14710</t>
+  </si>
+  <si>
+    <t>9468</t>
+  </si>
+  <si>
+    <t>9323</t>
+  </si>
+  <si>
+    <t>9070</t>
+  </si>
+  <si>
+    <t>8794</t>
+  </si>
+  <si>
+    <t>8503</t>
+  </si>
+  <si>
+    <t>20641</t>
+  </si>
+  <si>
+    <t>20868</t>
+  </si>
+  <si>
+    <t>20809</t>
+  </si>
+  <si>
+    <t>20951</t>
+  </si>
+  <si>
+    <t>21246</t>
   </si>
 </sst>
 </file>

</xml_diff>